<commit_message>
root cause with matching phrases from a different excel sheet
</commit_message>
<xml_diff>
--- a/Excel sheets/Sheet1.xlsx
+++ b/Excel sheets/Sheet1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a12a3dfde7402925/Documentos/Programming/Python/project/Excel sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a12a3dfde7402925/Documentos/Programming/Python/Root Cause Analysis/Excel sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{B73C68D5-24A0-41CC-9596-70B7EA3EE8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{324D029F-67AD-44B5-A35C-43FDD8650BB7}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{B73C68D5-24A0-41CC-9596-70B7EA3EE8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B866370-5602-4AAB-926C-B83AF51A8571}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C8F818BA-71CA-4D73-872B-D877EA82F99F}"/>
+    <workbookView xWindow="0" yWindow="10690" windowWidth="19420" windowHeight="10300" xr2:uid="{C8F818BA-71CA-4D73-872B-D877EA82F99F}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Material</t>
   </si>
@@ -69,6 +69,40 @@
   </si>
   <si>
     <t>Machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event:
+Process control
+Supplier didn't add the issue number to the board because they didn't know that they had to do this
+</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Machine
+Hello
+E-data</t>
+  </si>
+  <si>
+    <t>Material
+Repair</t>
+  </si>
+  <si>
+    <t>Human Error
+Repair</t>
   </si>
 </sst>
 </file>
@@ -104,8 +138,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,10 +161,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -444,107 +480,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B6E730-F4DA-4164-9AAF-B816342DBA1E}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>123456</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E10" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>